<commit_message>
Minor adaptations in translation tables
</commit_message>
<xml_diff>
--- a/Config/AllLocations.xlsx
+++ b/Config/AllLocations.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tabelle1!$A$1:$K$263</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -2932,6 +2935,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2940,49 +2947,49 @@
   <dimension ref="A1:K263"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3506,7 +3513,7 @@
         <v>71</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>72</v>
@@ -3982,7 +3989,7 @@
         <v>130</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>130</v>
@@ -9508,7 +9515,7 @@
         <v>747</v>
       </c>
       <c r="F211" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G211" s="0" t="s">
         <v>747</v>
@@ -11095,6 +11102,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K263"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -11102,5 +11110,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>